<commit_message>
adds and modifies vocabulary files
</commit_message>
<xml_diff>
--- a/resources/01 Verbs.xlsx
+++ b/resources/01 Verbs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arana/Dropbox/projects/education/languages/deutsch/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vvj0003/projects/education/deutsch/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA45152-CAE8-A14A-AFF6-EA554063001E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E02BC0-2249-6148-BED5-10A2A2E29B93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="440" windowWidth="16800" windowHeight="20560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verbs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="226">
   <si>
     <t>esse</t>
   </si>
@@ -120,12 +120,6 @@
     <t>read</t>
   </si>
   <si>
-    <t xml:space="preserve">sehen </t>
-  </si>
-  <si>
-    <t>see</t>
-  </si>
-  <si>
     <t>bringen</t>
   </si>
   <si>
@@ -312,12 +306,6 @@
     <t>to sell</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>we</t>
-  </si>
-  <si>
     <t>heißen</t>
   </si>
   <si>
@@ -348,21 +336,12 @@
     <t>think</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>verb</t>
   </si>
   <si>
     <t>meaning</t>
   </si>
   <si>
-    <t>you</t>
-  </si>
-  <si>
-    <t>they</t>
-  </si>
-  <si>
     <t>brauche</t>
   </si>
   <si>
@@ -798,21 +777,6 @@
     <t>probiert</t>
   </si>
   <si>
-    <t>sehe</t>
-  </si>
-  <si>
-    <t>siehst</t>
-  </si>
-  <si>
-    <t>sieht</t>
-  </si>
-  <si>
-    <t>sehen</t>
-  </si>
-  <si>
-    <t>seht</t>
-  </si>
-  <si>
     <t>spiele</t>
   </si>
   <si>
@@ -873,17 +837,271 @@
     <t>er/sie/es</t>
   </si>
   <si>
-    <t>you2</t>
-  </si>
-  <si>
-    <t>you3</t>
+    <t>to stand</t>
+  </si>
+  <si>
+    <t>wir</t>
+  </si>
+  <si>
+    <t>ich</t>
+  </si>
+  <si>
+    <t>du</t>
+  </si>
+  <si>
+    <t>ihr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sie </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>steh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>en</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>steh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>steh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>st</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>steh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>steh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>en</t>
+    </r>
+  </si>
+  <si>
+    <t>to see</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>seh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">en </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>seh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e</t>
+    </r>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>ˈzeːən</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>sieh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>st</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>sieh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>seh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>en</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>seh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -903,6 +1121,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -925,10 +1157,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1110,19 +1345,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15FB47A6-AE4F-6D4C-A536-2954825B74E1}" name="Table1" displayName="Table1" ref="A1:J50" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:J50" xr:uid="{44931CFB-BC3A-3F4E-96BD-263CD9705C08}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15FB47A6-AE4F-6D4C-A536-2954825B74E1}" name="Table1" displayName="Table1" ref="A1:J51" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:J51" xr:uid="{44931CFB-BC3A-3F4E-96BD-263CD9705C08}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J51">
+    <sortCondition ref="A1:A51"/>
+  </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{3DE7D73C-FCAF-9549-ABE5-C17CDC1929DB}" name="id"/>
     <tableColumn id="2" xr3:uid="{E4B399BA-18EE-7B45-A60A-87FA488B3B21}" name="verb"/>
     <tableColumn id="3" xr3:uid="{FACD9D36-D07A-CE42-A4CD-8531722F73DA}" name="meaning"/>
-    <tableColumn id="4" xr3:uid="{9DD5FA8E-517A-B34A-8E93-4BAC79AA1848}" name="I" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{98CB7397-6AE1-834C-8CE9-CC7CCA817C4D}" name="you" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{2F8947FC-B68B-B04F-8C8D-7287EF2AFC3B}" name="er/sie/es" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{5B3944E8-4B58-C544-8AC0-153C825BD8C3}" name="we" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{8A690D01-306C-734A-86CC-8B5EACF247F1}" name="you2" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{7E1AC344-8EAC-5046-8C1A-869B4F9C5D37}" name="you3" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{6F6C415D-F434-5A48-A9C8-5621C8D34D81}" name="they" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C01E427A-7481-7041-AE7A-29D451F2A633}" name="IPA"/>
+    <tableColumn id="4" xr3:uid="{9DD5FA8E-517A-B34A-8E93-4BAC79AA1848}" name="ich" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{98CB7397-6AE1-834C-8CE9-CC7CCA817C4D}" name="du" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{2F8947FC-B68B-B04F-8C8D-7287EF2AFC3B}" name="er/sie/es" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{5B3944E8-4B58-C544-8AC0-153C825BD8C3}" name="wir" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{8A690D01-306C-734A-86CC-8B5EACF247F1}" name="ihr" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{7E1AC344-8EAC-5046-8C1A-869B4F9C5D37}" name="Sie" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{6F6C415D-F434-5A48-A9C8-5621C8D34D81}" name="sie " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1449,106 +1687,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
+        <v>220</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1558,15 +1786,12 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1576,75 +1801,66 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" t="s">
-        <v>100</v>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1654,15 +1870,12 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>0</v>
@@ -1676,78 +1889,69 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>189</v>
       </c>
       <c r="B10" t="s">
-        <v>201</v>
-      </c>
-      <c r="C10" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D10" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="E10" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="F10" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="G10" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="H10" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="I10" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="J10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>81</v>
       </c>
       <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="G11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="I11" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="2"/>
@@ -1758,71 +1962,62 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>60</v>
       </c>
       <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1832,159 +2027,138 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>177</v>
       </c>
       <c r="B16" t="s">
-        <v>184</v>
-      </c>
-      <c r="C16" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>166</v>
       </c>
       <c r="B17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F17" t="s">
+        <v>170</v>
+      </c>
+      <c r="G17" t="s">
+        <v>166</v>
+      </c>
+      <c r="H17" t="s">
+        <v>170</v>
+      </c>
+      <c r="I17" t="s">
+        <v>166</v>
+      </c>
+      <c r="J17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F21" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D17" t="s">
+      <c r="G21" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F17" t="s">
-        <v>177</v>
-      </c>
-      <c r="G17" t="s">
-        <v>173</v>
-      </c>
-      <c r="H17" t="s">
-        <v>177</v>
-      </c>
-      <c r="I17" t="s">
-        <v>173</v>
-      </c>
-      <c r="J17" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>160</v>
-      </c>
-      <c r="C20" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="H21" s="2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="2"/>
@@ -1995,14 +2169,11 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>22</v>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="s">
         <v>30</v>
       </c>
       <c r="D23" s="2"/>
@@ -2013,53 +2184,47 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>23</v>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>160</v>
       </c>
       <c r="B24" t="s">
-        <v>167</v>
-      </c>
-      <c r="C24" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -2071,60 +2236,54 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>101</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>26</v>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>27</v>
@@ -2133,21 +2292,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>27</v>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -2155,110 +2311,98 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>28</v>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>181</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
-      </c>
-      <c r="C29" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>29</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>155</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
-      </c>
-      <c r="C30" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D30" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E30" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="F30" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="G30" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H30" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="I30" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J30" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>30</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>31</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" t="s">
         <v>16</v>
       </c>
       <c r="D32" s="2"/>
@@ -2269,46 +2413,40 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>32</v>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>33</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" t="s">
         <v>18</v>
       </c>
       <c r="D34" s="2"/>
@@ -2319,30 +2457,27 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>34</v>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" t="s">
         <v>26</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>25</v>
@@ -2351,15 +2486,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2369,47 +2501,44 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>36</v>
+    <row r="37" spans="1:10">
+      <c r="A37" t="s">
+        <v>218</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>217</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>221</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>193</v>
+        <v>219</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>195</v>
+        <v>223</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>51</v>
+        <v>224</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>37</v>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>6</v>
@@ -2430,63 +2559,57 @@
         <v>9</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>38</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" t="s">
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>39</v>
+    <row r="40" spans="1:10">
+      <c r="A40" t="s">
+        <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>13</v>
@@ -2495,307 +2618,306 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41">
+    <row r="41" spans="1:10">
+      <c r="A41" t="s">
+        <v>212</v>
+      </c>
+      <c r="B41" t="s">
+        <v>206</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" t="s">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" t="s">
+        <v>194</v>
+      </c>
+      <c r="B48" t="s">
+        <v>195</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" t="s">
+        <v>75</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E42" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" t="s">
-        <v>94</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46" t="s">
-        <v>42</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>206</v>
-      </c>
-      <c r="C47" t="s">
-        <v>207</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" t="s">
-        <v>36</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>76</v>
-      </c>
-      <c r="C49" t="s">
-        <v>77</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="H50" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
         <v>21</v>
       </c>
-      <c r="C50" t="s">
+      <c r="B51" t="s">
         <v>22</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="G50" s="2" t="s">
+      <c r="D51" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="I50" s="2" t="s">
+      <c r="H51" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J50" s="2" t="s">
+      <c r="J51" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2816,7 +2938,7 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2831,7 +2953,7 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>